<commit_message>
Updated XLSX data structures to include datacentre name for properties
</commit_message>
<xml_diff>
--- a/tests/Examples/TestDataWorkbook-1.xlsx
+++ b/tests/Examples/TestDataWorkbook-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>DataCentreName</t>
   </si>
@@ -642,7 +642,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,70 +800,86 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -874,71 +890,86 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>24</v>
       </c>
     </row>

</xml_diff>